<commit_message>
Files for major revision of Chapter 4b
</commit_message>
<xml_diff>
--- a/data/Ch4b/KY_Co_to_ADD.xlsx
+++ b/data/Ch4b/KY_Co_to_ADD.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\JuergenMicromapBook\RProjectFIle\MicromapPlotsInR-master\data\Ch4b\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74B92CF1-28B7-4AAC-B8DB-3F2191E027A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E9AB521-5AA8-4625-802A-E5DB83D8E442}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E919B24F-7254-4FDD-A0D9-C033FD421B0A}"/>
   </bookViews>
@@ -433,9 +433,6 @@
     <t>ID</t>
   </si>
   <si>
-    <t>County</t>
-  </si>
-  <si>
     <t>ADD</t>
   </si>
   <si>
@@ -449,6 +446,9 @@
   </si>
   <si>
     <t>Metcalfe</t>
+  </si>
+  <si>
+    <t>Name</t>
   </si>
 </sst>
 </file>
@@ -821,7 +821,7 @@
   <dimension ref="A1:C121"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -832,10 +832,10 @@
   <sheetData>
     <row r="1" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>132</v>
+        <v>137</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>131</v>
@@ -997,7 +997,7 @@
     </row>
     <row r="16" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>82</v>
@@ -1404,7 +1404,7 @@
     </row>
     <row r="53" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B53" s="2" t="s">
         <v>83</v>
@@ -1448,7 +1448,7 @@
     </row>
     <row r="57" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B57" s="2" t="s">
         <v>84</v>
@@ -1517,7 +1517,7 @@
         <v>10</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C63" s="1">
         <v>94</v>
@@ -1737,7 +1737,7 @@
         <v>0</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C83" s="1">
         <v>9</v>
@@ -1770,7 +1770,7 @@
         <v>1</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C86" s="1">
         <v>12</v>
@@ -1855,7 +1855,7 @@
     </row>
     <row r="94" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A94" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B94" s="2" t="s">
         <v>85</v>
@@ -1998,7 +1998,7 @@
     </row>
     <row r="107" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A107" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B107" s="2" t="s">
         <v>86</v>
@@ -2020,7 +2020,7 @@
     </row>
     <row r="109" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A109" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B109" s="2" t="s">
         <v>87</v>
@@ -2064,7 +2064,7 @@
     </row>
     <row r="113" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A113" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B113" s="2" t="s">
         <v>88</v>

</xml_diff>